<commit_message>
color change in dashboard
</commit_message>
<xml_diff>
--- a/college-list.xlsx
+++ b/college-list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="801">
   <si>
     <t>Karnataka</t>
   </si>
@@ -3120,12 +3120,69 @@
   <si>
     <t>IIT Gandhinagar</t>
   </si>
+  <si>
+    <t>GD Rungta College of Engineering and Technology (GDRCET) , Bhilai</t>
+  </si>
+  <si>
+    <t>Bharath university , Chennai</t>
+  </si>
+  <si>
+    <t>Thapar University , Patiala</t>
+  </si>
+  <si>
+    <t>Jai Prakash University (JP), Chapra</t>
+  </si>
+  <si>
+    <t>Chapra</t>
+  </si>
+  <si>
+    <t>Assam Don Bosco University - Azara Campus , Guwahati</t>
+  </si>
+  <si>
+    <t>Babulal Tarabai Institute of Research and Technology (BTIRT), Sagar</t>
+  </si>
+  <si>
+    <t>Sagar</t>
+  </si>
+  <si>
+    <t>Anand Engineering College (AEC) , Agra</t>
+  </si>
+  <si>
+    <t>PDM College of Engineering (PDMCE) , Bahadurgarh</t>
+  </si>
+  <si>
+    <t>Bahadurgarh</t>
+  </si>
+  <si>
+    <t>Government Model Engineering College (MEC) , Kochi</t>
+  </si>
+  <si>
+    <t>International Institute of Information Technology (IIIT), Bhubaneswar</t>
+  </si>
+  <si>
+    <t>Ideal Institute of Technology , Ghaziabad</t>
+  </si>
+  <si>
+    <t>Delhi Institute of Tool Engineering , Delhi</t>
+  </si>
+  <si>
+    <t>National Institute of Technology (NIT) , Delhi</t>
+  </si>
+  <si>
+    <t>IGNOU , MUZZAFARPUR</t>
+  </si>
+  <si>
+    <t>IGNOU , Delhi</t>
+  </si>
+  <si>
+    <t>MBICEM GGSIPU , DELHI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3165,6 +3222,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3192,13 +3255,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3503,10 +3567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F553"/>
+  <dimension ref="A1:F569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A537" workbookViewId="0">
-      <selection activeCell="B553" sqref="B553"/>
+    <sheetView tabSelected="1" topLeftCell="A547" workbookViewId="0">
+      <selection activeCell="A570" sqref="A570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12720,7 +12784,7 @@
         <v>719</v>
       </c>
       <c r="B512" t="str">
-        <f t="shared" ref="B512:B553" si="10">UPPER(A512)</f>
+        <f t="shared" ref="B512:B569" si="10">UPPER(A512)</f>
         <v>VIMAL JYOTHI ENGINEERING COLLEGE, KANNUR</v>
       </c>
       <c r="C512">
@@ -13469,6 +13533,294 @@
       </c>
       <c r="F553" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>782</v>
+      </c>
+      <c r="B554" t="str">
+        <f t="shared" si="10"/>
+        <v>GD RUNGTA COLLEGE OF ENGINEERING AND TECHNOLOGY (GDRCET) , BHILAI</v>
+      </c>
+      <c r="C554">
+        <v>557</v>
+      </c>
+      <c r="E554" t="s">
+        <v>181</v>
+      </c>
+      <c r="F554" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>783</v>
+      </c>
+      <c r="B555" t="str">
+        <f t="shared" si="10"/>
+        <v>BHARATH UNIVERSITY , CHENNAI</v>
+      </c>
+      <c r="C555">
+        <v>558</v>
+      </c>
+      <c r="E555" t="s">
+        <v>59</v>
+      </c>
+      <c r="F555" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>784</v>
+      </c>
+      <c r="B556" t="str">
+        <f t="shared" si="10"/>
+        <v>THAPAR UNIVERSITY , PATIALA</v>
+      </c>
+      <c r="C556">
+        <v>559</v>
+      </c>
+      <c r="E556" t="s">
+        <v>301</v>
+      </c>
+      <c r="F556" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>785</v>
+      </c>
+      <c r="B557" t="str">
+        <f t="shared" si="10"/>
+        <v>JAI PRAKASH UNIVERSITY (JP), CHAPRA</v>
+      </c>
+      <c r="C557">
+        <v>560</v>
+      </c>
+      <c r="E557" t="s">
+        <v>786</v>
+      </c>
+      <c r="F557" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>787</v>
+      </c>
+      <c r="B558" t="str">
+        <f t="shared" si="10"/>
+        <v>ASSAM DON BOSCO UNIVERSITY - AZARA CAMPUS , GUWAHATI</v>
+      </c>
+      <c r="C558">
+        <v>561</v>
+      </c>
+      <c r="E558" t="s">
+        <v>19</v>
+      </c>
+      <c r="F558" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A559" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="B559" t="str">
+        <f t="shared" si="10"/>
+        <v>BABULAL TARABAI INSTITUTE OF RESEARCH AND TECHNOLOGY (BTIRT), SAGAR</v>
+      </c>
+      <c r="C559">
+        <v>562</v>
+      </c>
+      <c r="E559" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="F559" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A560" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="B560" t="str">
+        <f t="shared" si="10"/>
+        <v>ANAND ENGINEERING COLLEGE (AEC) , AGRA</v>
+      </c>
+      <c r="C560">
+        <v>563</v>
+      </c>
+      <c r="E560" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F560" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A561" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="B561" t="str">
+        <f t="shared" si="10"/>
+        <v>PDM COLLEGE OF ENGINEERING (PDMCE) , BAHADURGARH</v>
+      </c>
+      <c r="C561">
+        <v>564</v>
+      </c>
+      <c r="E561" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="F561" s="4" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A562" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="B562" t="str">
+        <f t="shared" si="10"/>
+        <v>GOVERNMENT MODEL ENGINEERING COLLEGE (MEC) , KOCHI</v>
+      </c>
+      <c r="C562">
+        <v>565</v>
+      </c>
+      <c r="E562" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="F562" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A563" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="B563" t="str">
+        <f t="shared" si="10"/>
+        <v>INTERNATIONAL INSTITUTE OF INFORMATION TECHNOLOGY (IIIT), BHUBANESWAR</v>
+      </c>
+      <c r="C563">
+        <v>566</v>
+      </c>
+      <c r="E563" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F563" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A564" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="B564" t="str">
+        <f t="shared" si="10"/>
+        <v>IDEAL INSTITUTE OF TECHNOLOGY , GHAZIABAD</v>
+      </c>
+      <c r="C564">
+        <v>567</v>
+      </c>
+      <c r="E564" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F564" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A565" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="B565" t="str">
+        <f t="shared" si="10"/>
+        <v>DELHI INSTITUTE OF TOOL ENGINEERING , DELHI</v>
+      </c>
+      <c r="C565">
+        <v>568</v>
+      </c>
+      <c r="E565" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F565" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A566" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="B566" t="str">
+        <f t="shared" si="10"/>
+        <v>NATIONAL INSTITUTE OF TECHNOLOGY (NIT) , DELHI</v>
+      </c>
+      <c r="C566">
+        <v>569</v>
+      </c>
+      <c r="E566" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F566" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>798</v>
+      </c>
+      <c r="B567" t="str">
+        <f t="shared" si="10"/>
+        <v>IGNOU , MUZZAFARPUR</v>
+      </c>
+      <c r="C567">
+        <v>570</v>
+      </c>
+      <c r="E567" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="F567" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>799</v>
+      </c>
+      <c r="B568" t="str">
+        <f t="shared" si="10"/>
+        <v>IGNOU , DELHI</v>
+      </c>
+      <c r="C568">
+        <v>571</v>
+      </c>
+      <c r="E568" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F568" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>800</v>
+      </c>
+      <c r="B569" t="str">
+        <f t="shared" si="10"/>
+        <v>MBICEM GGSIPU , DELHI</v>
+      </c>
+      <c r="C569">
+        <v>572</v>
+      </c>
+      <c r="E569" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F569" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>